<commit_message>
Agregando la respuesta al sexto reto de programación.
</commit_message>
<xml_diff>
--- a/support.xlsx
+++ b/support.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\david\OneDrive\Documents\Proyectos\code_challenges\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3C361430-CA63-4782-BB9F-749BB7B7385F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52827BB9-FB28-4DFE-BBC0-3A24A0B8D008}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="1" xr2:uid="{F9BEF1A1-117A-42F5-99A3-FEFFC57AEB17}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="16440" windowHeight="28320" activeTab="2" xr2:uid="{F9BEF1A1-117A-42F5-99A3-FEFFC57AEB17}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
     <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="289" uniqueCount="111">
   <si>
     <t>A</t>
   </si>
@@ -752,7 +753,7 @@
         <v>29</v>
       </c>
       <c r="G15" t="str">
-        <f>LOWER(D15)</f>
+        <f t="shared" ref="G15:G41" si="0">LOWER(D15)</f>
         <v>a</v>
       </c>
       <c r="H15" t="str">
@@ -771,18 +772,18 @@
         <v>1</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" ref="E16:E41" si="0">CONCATENATE("'",D16,"'")</f>
+        <f t="shared" ref="E16:E41" si="1">CONCATENATE("'",D16,"'")</f>
         <v>'B'</v>
       </c>
       <c r="F16" t="s">
         <v>29</v>
       </c>
       <c r="G16" t="str">
-        <f>LOWER(D16)</f>
+        <f t="shared" si="0"/>
         <v>b</v>
       </c>
       <c r="H16" t="str">
-        <f t="shared" ref="H16:H41" si="1">CONCATENATE("'",G16,"'")</f>
+        <f t="shared" ref="H16:H41" si="2">CONCATENATE("'",G16,"'")</f>
         <v>'b'</v>
       </c>
       <c r="J16" t="s">
@@ -797,18 +798,18 @@
         <v>2</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'C'</v>
       </c>
       <c r="F17" t="s">
         <v>29</v>
       </c>
       <c r="G17" t="str">
-        <f>LOWER(D17)</f>
+        <f t="shared" si="0"/>
         <v>c</v>
       </c>
       <c r="H17" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'c'</v>
       </c>
       <c r="J17" t="s">
@@ -823,18 +824,18 @@
         <v>3</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'D'</v>
       </c>
       <c r="F18" t="s">
         <v>29</v>
       </c>
       <c r="G18" t="str">
-        <f>LOWER(D18)</f>
+        <f t="shared" si="0"/>
         <v>d</v>
       </c>
       <c r="H18" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'d'</v>
       </c>
       <c r="J18" t="s">
@@ -849,18 +850,18 @@
         <v>4</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'E'</v>
       </c>
       <c r="F19" t="s">
         <v>29</v>
       </c>
       <c r="G19" t="str">
-        <f>LOWER(D19)</f>
+        <f t="shared" si="0"/>
         <v>e</v>
       </c>
       <c r="H19" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'e'</v>
       </c>
       <c r="J19">
@@ -875,18 +876,18 @@
         <v>5</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'F'</v>
       </c>
       <c r="F20" t="s">
         <v>29</v>
       </c>
       <c r="G20" t="str">
-        <f>LOWER(D20)</f>
+        <f t="shared" si="0"/>
         <v>f</v>
       </c>
       <c r="H20" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'f'</v>
       </c>
       <c r="J20" t="s">
@@ -901,18 +902,18 @@
         <v>6</v>
       </c>
       <c r="E21" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'G'</v>
       </c>
       <c r="F21" t="s">
         <v>29</v>
       </c>
       <c r="G21" t="str">
-        <f>LOWER(D21)</f>
+        <f t="shared" si="0"/>
         <v>g</v>
       </c>
       <c r="H21" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'g'</v>
       </c>
       <c r="J21" t="s">
@@ -927,18 +928,18 @@
         <v>7</v>
       </c>
       <c r="E22" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'H'</v>
       </c>
       <c r="F22" t="s">
         <v>29</v>
       </c>
       <c r="G22" t="str">
-        <f>LOWER(D22)</f>
+        <f t="shared" si="0"/>
         <v>h</v>
       </c>
       <c r="H22" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'h'</v>
       </c>
       <c r="J22" t="s">
@@ -953,18 +954,18 @@
         <v>8</v>
       </c>
       <c r="E23" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'I'</v>
       </c>
       <c r="F23" t="s">
         <v>29</v>
       </c>
       <c r="G23" t="str">
-        <f>LOWER(D23)</f>
+        <f t="shared" si="0"/>
         <v>i</v>
       </c>
       <c r="H23" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'i'</v>
       </c>
       <c r="J23">
@@ -979,18 +980,18 @@
         <v>9</v>
       </c>
       <c r="E24" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'J'</v>
       </c>
       <c r="F24" t="s">
         <v>29</v>
       </c>
       <c r="G24" t="str">
-        <f>LOWER(D24)</f>
+        <f t="shared" si="0"/>
         <v>j</v>
       </c>
       <c r="H24" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'j'</v>
       </c>
       <c r="J24" t="s">
@@ -1005,18 +1006,18 @@
         <v>10</v>
       </c>
       <c r="E25" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'K'</v>
       </c>
       <c r="F25" t="s">
         <v>29</v>
       </c>
       <c r="G25" t="str">
-        <f>LOWER(D25)</f>
+        <f t="shared" si="0"/>
         <v>k</v>
       </c>
       <c r="H25" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'k'</v>
       </c>
       <c r="J25" t="s">
@@ -1031,18 +1032,18 @@
         <v>11</v>
       </c>
       <c r="E26" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'L'</v>
       </c>
       <c r="F26" t="s">
         <v>29</v>
       </c>
       <c r="G26" t="str">
-        <f>LOWER(D26)</f>
+        <f t="shared" si="0"/>
         <v>l</v>
       </c>
       <c r="H26" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'l'</v>
       </c>
       <c r="J26">
@@ -1057,18 +1058,18 @@
         <v>12</v>
       </c>
       <c r="E27" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'M'</v>
       </c>
       <c r="F27" t="s">
         <v>29</v>
       </c>
       <c r="G27" t="str">
-        <f>LOWER(D27)</f>
+        <f t="shared" si="0"/>
         <v>m</v>
       </c>
       <c r="H27" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'m'</v>
       </c>
       <c r="J27" t="s">
@@ -1083,18 +1084,18 @@
         <v>13</v>
       </c>
       <c r="E28" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'N'</v>
       </c>
       <c r="F28" t="s">
         <v>29</v>
       </c>
       <c r="G28" t="str">
-        <f>LOWER(D28)</f>
+        <f t="shared" si="0"/>
         <v>n</v>
       </c>
       <c r="H28" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'n'</v>
       </c>
       <c r="J28" t="s">
@@ -1109,18 +1110,18 @@
         <v>25</v>
       </c>
       <c r="E29" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'Ñ'</v>
       </c>
       <c r="F29" t="s">
         <v>29</v>
       </c>
       <c r="G29" t="str">
-        <f>LOWER(D29)</f>
+        <f t="shared" si="0"/>
         <v>ñ</v>
       </c>
       <c r="H29" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'ñ'</v>
       </c>
       <c r="J29" t="s">
@@ -1135,18 +1136,18 @@
         <v>14</v>
       </c>
       <c r="E30" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'O'</v>
       </c>
       <c r="F30" t="s">
         <v>29</v>
       </c>
       <c r="G30" t="str">
-        <f>LOWER(D30)</f>
+        <f t="shared" si="0"/>
         <v>o</v>
       </c>
       <c r="H30" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'o'</v>
       </c>
       <c r="J30">
@@ -1161,18 +1162,18 @@
         <v>15</v>
       </c>
       <c r="E31" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'P'</v>
       </c>
       <c r="F31" t="s">
         <v>29</v>
       </c>
       <c r="G31" t="str">
-        <f>LOWER(D31)</f>
+        <f t="shared" si="0"/>
         <v>p</v>
       </c>
       <c r="H31" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'p'</v>
       </c>
       <c r="J31" t="s">
@@ -1187,18 +1188,18 @@
         <v>16</v>
       </c>
       <c r="E32" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'Q'</v>
       </c>
       <c r="F32" t="s">
         <v>29</v>
       </c>
       <c r="G32" t="str">
-        <f>LOWER(D32)</f>
+        <f t="shared" si="0"/>
         <v>q</v>
       </c>
       <c r="H32" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'q'</v>
       </c>
       <c r="J32" t="s">
@@ -1213,18 +1214,18 @@
         <v>17</v>
       </c>
       <c r="E33" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'R'</v>
       </c>
       <c r="F33" t="s">
         <v>29</v>
       </c>
       <c r="G33" t="str">
-        <f>LOWER(D33)</f>
+        <f t="shared" si="0"/>
         <v>r</v>
       </c>
       <c r="H33" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'r'</v>
       </c>
       <c r="J33" t="s">
@@ -1239,18 +1240,18 @@
         <v>18</v>
       </c>
       <c r="E34" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'S'</v>
       </c>
       <c r="F34" t="s">
         <v>29</v>
       </c>
       <c r="G34" t="str">
-        <f>LOWER(D34)</f>
+        <f t="shared" si="0"/>
         <v>s</v>
       </c>
       <c r="H34" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'s'</v>
       </c>
       <c r="J34" t="s">
@@ -1265,18 +1266,18 @@
         <v>19</v>
       </c>
       <c r="E35" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'T'</v>
       </c>
       <c r="F35" t="s">
         <v>29</v>
       </c>
       <c r="G35" t="str">
-        <f>LOWER(D35)</f>
+        <f t="shared" si="0"/>
         <v>t</v>
       </c>
       <c r="H35" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'t'</v>
       </c>
       <c r="J35" t="s">
@@ -1291,18 +1292,18 @@
         <v>20</v>
       </c>
       <c r="E36" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'U'</v>
       </c>
       <c r="F36" t="s">
         <v>29</v>
       </c>
       <c r="G36" t="str">
-        <f>LOWER(D36)</f>
+        <f t="shared" si="0"/>
         <v>u</v>
       </c>
       <c r="H36" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'u'</v>
       </c>
       <c r="J36" t="s">
@@ -1317,18 +1318,18 @@
         <v>21</v>
       </c>
       <c r="E37" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'V'</v>
       </c>
       <c r="F37" t="s">
         <v>29</v>
       </c>
       <c r="G37" t="str">
-        <f>LOWER(D37)</f>
+        <f t="shared" si="0"/>
         <v>v</v>
       </c>
       <c r="H37" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'v'</v>
       </c>
       <c r="J37" t="s">
@@ -1343,18 +1344,18 @@
         <v>22</v>
       </c>
       <c r="E38" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'W'</v>
       </c>
       <c r="F38" t="s">
         <v>29</v>
       </c>
       <c r="G38" t="str">
-        <f>LOWER(D38)</f>
+        <f t="shared" si="0"/>
         <v>w</v>
       </c>
       <c r="H38" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'w'</v>
       </c>
       <c r="J38" t="s">
@@ -1369,18 +1370,18 @@
         <v>23</v>
       </c>
       <c r="E39" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'X'</v>
       </c>
       <c r="F39" t="s">
         <v>29</v>
       </c>
       <c r="G39" t="str">
-        <f>LOWER(D39)</f>
+        <f t="shared" si="0"/>
         <v>x</v>
       </c>
       <c r="H39" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'x'</v>
       </c>
       <c r="J39" t="s">
@@ -1395,18 +1396,18 @@
         <v>26</v>
       </c>
       <c r="E40" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'Y'</v>
       </c>
       <c r="F40" t="s">
         <v>29</v>
       </c>
       <c r="G40" t="str">
-        <f>LOWER(D40)</f>
+        <f t="shared" si="0"/>
         <v>y</v>
       </c>
       <c r="H40" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'y'</v>
       </c>
       <c r="J40" t="s">
@@ -1421,18 +1422,18 @@
         <v>24</v>
       </c>
       <c r="E41" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>'Z'</v>
       </c>
       <c r="F41" t="s">
         <v>29</v>
       </c>
       <c r="G41" t="str">
-        <f>LOWER(D41)</f>
+        <f t="shared" si="0"/>
         <v>z</v>
       </c>
       <c r="H41" t="str">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>'z'</v>
       </c>
       <c r="J41">
@@ -1449,7 +1450,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31402AFD-5592-4F82-AA45-35A0513540C4}">
   <dimension ref="B14:K40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K14" sqref="K14:K40"/>
     </sheetView>
   </sheetViews>
@@ -2305,4 +2306,55 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D63CB61-570D-42F6-9A46-BE1D0739E093}">
+  <dimension ref="C10:D15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="10" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C14">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C15">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>